<commit_message>
Process is verified and ready to run
</commit_message>
<xml_diff>
--- a/Regler.xlsx
+++ b/Regler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\RPA\Leverancer\Postmester Medcom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\RPA\Leverancer\Postmester Medcom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74CB5F6-F734-4A35-A8EE-5ED401018EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F737AF-C0C9-491A-97D8-171C1A0C8FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E3DC931-000A-4C90-ACC4-C77086F852B4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7E3DC931-000A-4C90-ACC4-C77086F852B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Regler" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
 MedCom</t>
   </si>
   <si>
-    <t>Rehabilitering og Palliation</t>
-  </si>
-  <si>
     <t>Korrespondance: Kommunikationscenter Odense</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
     <t>Sundhedsfagligt grundforløb/FSIII
 MedCom
 Sundhedsfagligt grundforløb/Korrespondance - Sundhed og forebyggelse</t>
+  </si>
+  <si>
+    <t>Rehabilitering og palliation</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,19 +547,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -573,53 +573,53 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -670,7 +670,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -678,165 +678,165 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -859,7 +859,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>